<commit_message>
updates with new data for eipes
</commit_message>
<xml_diff>
--- a/by_specialty.xlsx
+++ b/by_specialty.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">specialty</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">ΠΑΙΔΙΑΤΡΙΚΗ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΠΛΑΣΤΙΚΗ, ΕΠΑΝΟΡΘΩΤΙΚΗ ΚΑΙ ΑΙΣΘΗΤΙΚΗ ΧΕΙΡΟΥΡΓΙΚΗ</t>
   </si>
   <si>
     <t xml:space="preserve">ΠΝΕΥΜΟΝΟΛΟΓΙΑ - ΦΥΜΑΤΙΟΛΟΓΙΑ</t>
@@ -466,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" t="n">
         <v>0.07</v>
@@ -488,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
         <v>0.02</v>
@@ -499,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
         <v>0.03</v>
@@ -510,7 +513,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
         <v>0.03</v>
@@ -521,10 +524,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9">
@@ -532,10 +535,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="10">
@@ -543,7 +546,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="n">
         <v>0.02</v>
@@ -565,10 +568,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13">
@@ -576,7 +579,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C13" t="n">
         <v>0.07</v>
@@ -587,10 +590,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="15">
@@ -598,7 +601,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C15" t="n">
         <v>0.08</v>
@@ -609,7 +612,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" t="n">
         <v>0.03</v>
@@ -620,7 +623,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C17" t="n">
         <v>0.04</v>
@@ -631,7 +634,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
         <v>0.02</v>
@@ -642,7 +645,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" t="n">
         <v>0.03</v>
@@ -653,7 +656,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
         <v>0.02</v>
@@ -664,10 +667,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22">
@@ -675,7 +678,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C22" t="n">
         <v>0.07</v>
@@ -686,10 +689,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -697,10 +700,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25">
@@ -708,10 +711,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C25" t="n">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="26">
@@ -719,10 +722,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27">
@@ -730,10 +733,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -741,10 +744,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>0.22</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="29">
@@ -752,10 +755,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="C29" t="n">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="30">
@@ -763,9 +766,20 @@
         <v>31</v>
       </c>
       <c r="B30" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C30" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="n">
+        <v>7</v>
+      </c>
+      <c r="C31" t="n">
         <v>0.02</v>
       </c>
     </row>

</xml_diff>

<commit_message>
further changes to various
</commit_message>
<xml_diff>
--- a/by_specialty.xlsx
+++ b/by_specialty.xlsx
@@ -458,7 +458,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
         <v>0.01</v>
@@ -469,10 +469,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="n">
-        <v>0.07</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="4">
@@ -513,7 +513,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>0.03</v>
@@ -524,10 +524,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="9">
@@ -560,7 +560,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12">
@@ -579,10 +579,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="n">
-        <v>0.07</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="14">
@@ -593,7 +593,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="15">
@@ -601,10 +601,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C15" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="16">
@@ -612,7 +612,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" t="n">
         <v>0.03</v>
@@ -623,7 +623,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" t="n">
         <v>0.04</v>
@@ -634,10 +634,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C18" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="19">
@@ -645,7 +645,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C19" t="n">
         <v>0.03</v>
@@ -678,10 +678,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C22" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="23">
@@ -700,7 +700,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C24" t="n">
         <v>0.02</v>
@@ -725,7 +725,7 @@
         <v>16</v>
       </c>
       <c r="C26" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="27">
@@ -733,10 +733,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28">
@@ -755,7 +755,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C29" t="n">
         <v>0.2</v>
@@ -777,10 +777,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C31" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>